<commit_message>
actualiza los valores en lista
</commit_message>
<xml_diff>
--- a/Código de Ética - Hospital Roberto del Río (Respuestas).xlsx
+++ b/Código de Ética - Hospital Roberto del Río (Respuestas).xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\auditoria1\Desktop\Mis documentos\2022\SISTEMA DE INTEGRIDAD\AÑO 2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\control.gestion3\Documents\GitHub\Encuesta_Etica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01919C8-9C40-4DDE-986C-E5B1058DDAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Respuestas de formulario 1'!$AJ$1:$AM$301</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10535" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10735" uniqueCount="633">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1805,15 +1807,144 @@
   <si>
     <t>Compra de insumos que poco o no son de mejor uso en nuestros pacientes.</t>
   </si>
+  <si>
+    <t>Licencias medicas</t>
+  </si>
+  <si>
+    <t>Discriminación a pacientes</t>
+  </si>
+  <si>
+    <t>No cumplen jornada laboral</t>
+  </si>
+  <si>
+    <t>Conflicto de interes</t>
+  </si>
+  <si>
+    <t>Mal uso de recursos públicos</t>
+  </si>
+  <si>
+    <t>Deshonestidad</t>
+  </si>
+  <si>
+    <t>Discriminación laboral</t>
+  </si>
+  <si>
+    <t>Concursos públicos</t>
+  </si>
+  <si>
+    <t>Buena atención</t>
+  </si>
+  <si>
+    <t>Horas extras</t>
+  </si>
+  <si>
+    <t>Falta de control de jefatura</t>
+  </si>
+  <si>
+    <t>Ingreso irregular a la institución</t>
+  </si>
+  <si>
+    <t>Denuncias falsas</t>
+  </si>
+  <si>
+    <t>Maltrato laboral</t>
+  </si>
+  <si>
+    <t>Notratno heboral</t>
+  </si>
+  <si>
+    <t>Acoso laboral</t>
+  </si>
+  <si>
+    <t>Sumarios sin sanción</t>
+  </si>
+  <si>
+    <t>Actividades administrativas mal ejecutadas</t>
+  </si>
+  <si>
+    <t>Probidad</t>
+  </si>
+  <si>
+    <t>Discusiones profesionales</t>
+  </si>
+  <si>
+    <t>Interes personal sobre el colectivo</t>
+  </si>
+  <si>
+    <t>SDGP</t>
+  </si>
+  <si>
+    <t>Atención deficiente</t>
+  </si>
+  <si>
+    <t>Licencias Medicas</t>
+  </si>
+  <si>
+    <t>Atención a pacientes deficiente</t>
+  </si>
+  <si>
+    <t>Vulneración de derechos del paciente</t>
+  </si>
+  <si>
+    <t>Aprovechamiento de atención por funcionarios</t>
+  </si>
+  <si>
+    <t>Falta de compromiso en la atención</t>
+  </si>
+  <si>
+    <t>Trabajo administrativo mal ejecutado</t>
+  </si>
+  <si>
+    <t>Honestidad</t>
+  </si>
+  <si>
+    <t>Transparencia</t>
+  </si>
+  <si>
+    <t>Relación con proveedores</t>
+  </si>
+  <si>
+    <t>No ejecuta trabajo</t>
+  </si>
+  <si>
+    <t>Acusaciones falsas</t>
+  </si>
+  <si>
+    <t>Falta de calidad en la atención</t>
+  </si>
+  <si>
+    <t>Trabajo en equipo deficiente</t>
+  </si>
+  <si>
+    <t>Acoso sexual</t>
+  </si>
+  <si>
+    <t>Rumores</t>
+  </si>
+  <si>
+    <t>Mejora de grados</t>
+  </si>
+  <si>
+    <t>Abuso de poder</t>
+  </si>
+  <si>
+    <t>cat 1</t>
+  </si>
+  <si>
+    <t>cat 2</t>
+  </si>
+  <si>
+    <t>cat 3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1824,6 +1955,20 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1847,12 +1992,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2067,23 +2214,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ301"/>
+  <dimension ref="A1:AM301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="AL147" sqref="AL147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="42" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="35" width="18.85546875" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="112.85546875" customWidth="1"/>
+    <col min="37" max="42" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2192,8 +2342,17 @@
       <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="AK1" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>632</v>
+      </c>
     </row>
-    <row r="2" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>44700.52952866898</v>
       </c>
@@ -2302,8 +2461,11 @@
       <c r="AJ2" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="AK2" s="2" t="s">
+        <v>590</v>
+      </c>
     </row>
-    <row r="3" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>44700.531511157409</v>
       </c>
@@ -2412,8 +2574,11 @@
       <c r="AJ3" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="AK3" s="2" t="s">
+        <v>591</v>
+      </c>
     </row>
-    <row r="4" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>44700.533345636577</v>
       </c>
@@ -2522,8 +2687,11 @@
       <c r="AJ4" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="AK4" s="5" t="s">
+        <v>618</v>
+      </c>
     </row>
-    <row r="5" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>44700.53520888889</v>
       </c>
@@ -2629,11 +2797,11 @@
       <c r="AI5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AJ5" s="2" t="s">
+      <c r="AJ5" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>44700.536423831014</v>
       </c>
@@ -2739,11 +2907,11 @@
       <c r="AI6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AJ6" s="2" t="s">
+      <c r="AJ6" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>44700.542387777779</v>
       </c>
@@ -2852,8 +3020,11 @@
       <c r="AJ7" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="AK7" s="2" t="s">
+        <v>592</v>
+      </c>
     </row>
-    <row r="8" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>44700.545561273146</v>
       </c>
@@ -2959,11 +3130,11 @@
       <c r="AI8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AJ8" s="2" t="s">
+      <c r="AJ8" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>44700.552090081022</v>
       </c>
@@ -3072,8 +3243,11 @@
       <c r="AJ9" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="AK9" s="2" t="s">
+        <v>593</v>
+      </c>
     </row>
-    <row r="10" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>44700.553169363426</v>
       </c>
@@ -3182,8 +3356,11 @@
       <c r="AJ10" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="AK10" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="11" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>44700.554673680555</v>
       </c>
@@ -3292,8 +3469,11 @@
       <c r="AJ11" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="AK11" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="12" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>44700.560503078705</v>
       </c>
@@ -3399,11 +3579,11 @@
       <c r="AI12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AJ12" s="2" t="s">
+      <c r="AJ12" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>44700.561590532408</v>
       </c>
@@ -3512,8 +3692,11 @@
       <c r="AJ13" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="AK13" s="2" t="s">
+        <v>595</v>
+      </c>
     </row>
-    <row r="14" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>44700.562803252316</v>
       </c>
@@ -3622,8 +3805,11 @@
       <c r="AJ14" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="AK14" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="15" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>44700.56501179398</v>
       </c>
@@ -3732,8 +3918,11 @@
       <c r="AJ15" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="AK15" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="16" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>44700.568405729166</v>
       </c>
@@ -3842,8 +4031,11 @@
       <c r="AJ16" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="AK16" s="2" t="s">
+        <v>596</v>
+      </c>
     </row>
-    <row r="17" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>44700.568447118058</v>
       </c>
@@ -3949,11 +4141,11 @@
       <c r="AI17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AJ17" s="2" t="s">
+      <c r="AJ17" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>44700.570475358792</v>
       </c>
@@ -4062,8 +4254,11 @@
       <c r="AJ18" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="AK18" s="2" t="s">
+        <v>597</v>
+      </c>
     </row>
-    <row r="19" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>44700.572380949074</v>
       </c>
@@ -4172,8 +4367,11 @@
       <c r="AJ19" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="AK19" s="2" t="s">
+        <v>601</v>
+      </c>
     </row>
-    <row r="20" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>44700.572532164355</v>
       </c>
@@ -4279,11 +4477,11 @@
       <c r="AI20" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AJ20" s="2" t="s">
+      <c r="AJ20" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>44700.572728761574</v>
       </c>
@@ -4392,8 +4590,11 @@
       <c r="AJ21" s="2" t="s">
         <v>84</v>
       </c>
+      <c r="AK21" s="2" t="s">
+        <v>598</v>
+      </c>
     </row>
-    <row r="22" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>44700.583278483798</v>
       </c>
@@ -4499,11 +4700,11 @@
       <c r="AI22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AJ22" s="2" t="s">
+      <c r="AJ22" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>44700.594424907409</v>
       </c>
@@ -4612,8 +4813,11 @@
       <c r="AJ23" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="AK23" s="2" t="s">
+        <v>597</v>
+      </c>
     </row>
-    <row r="24" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>44700.594679178241</v>
       </c>
@@ -4722,8 +4926,14 @@
       <c r="AJ24" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="AK24" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AL24" s="2" t="s">
+        <v>599</v>
+      </c>
     </row>
-    <row r="25" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>44700.605132627315</v>
       </c>
@@ -4829,11 +5039,11 @@
       <c r="AI25" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AJ25" s="2" t="s">
+      <c r="AJ25" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>44700.607098055552</v>
       </c>
@@ -4942,8 +5152,11 @@
       <c r="AJ26" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="AK26" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="27" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>44700.607113217593</v>
       </c>
@@ -5052,8 +5265,11 @@
       <c r="AJ27" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="AK27" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="28" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>44700.60770552083</v>
       </c>
@@ -5162,8 +5378,11 @@
       <c r="AJ28" s="2" t="s">
         <v>98</v>
       </c>
+      <c r="AK28" s="2" t="s">
+        <v>599</v>
+      </c>
     </row>
-    <row r="29" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>44700.61003851852</v>
       </c>
@@ -5272,8 +5491,14 @@
       <c r="AJ29" s="2" t="s">
         <v>100</v>
       </c>
+      <c r="AK29" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AL29" s="2" t="s">
+        <v>600</v>
+      </c>
     </row>
-    <row r="30" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>44700.615209849537</v>
       </c>
@@ -5382,8 +5607,11 @@
       <c r="AJ30" s="2" t="s">
         <v>102</v>
       </c>
+      <c r="AK30" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="31" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>44700.642805682874</v>
       </c>
@@ -5492,8 +5720,11 @@
       <c r="AJ31" s="2" t="s">
         <v>104</v>
       </c>
+      <c r="AK31" s="2" t="s">
+        <v>592</v>
+      </c>
     </row>
-    <row r="32" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:39" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>44700.646956342593</v>
       </c>
@@ -5602,8 +5833,17 @@
       <c r="AJ32" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="AK32" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AL32" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="AM32" s="2" t="s">
+        <v>611</v>
+      </c>
     </row>
-    <row r="33" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>44700.651915416667</v>
       </c>
@@ -5712,8 +5952,11 @@
       <c r="AJ33" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="AK33" s="2" t="s">
+        <v>599</v>
+      </c>
     </row>
-    <row r="34" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>44700.664048206017</v>
       </c>
@@ -5822,8 +6065,11 @@
       <c r="AJ34" s="2" t="s">
         <v>110</v>
       </c>
+      <c r="AK34" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="35" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>44700.679212835646</v>
       </c>
@@ -5932,8 +6178,11 @@
       <c r="AJ35" s="2" t="s">
         <v>112</v>
       </c>
+      <c r="AK35" s="2" t="s">
+        <v>602</v>
+      </c>
     </row>
-    <row r="36" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>44700.688107615744</v>
       </c>
@@ -6042,8 +6291,11 @@
       <c r="AJ36" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="AK36" s="2" t="s">
+        <v>601</v>
+      </c>
     </row>
-    <row r="37" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>44700.690522777775</v>
       </c>
@@ -6152,8 +6404,14 @@
       <c r="AJ37" s="2" t="s">
         <v>116</v>
       </c>
+      <c r="AK37" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AL37" s="2" t="s">
+        <v>599</v>
+      </c>
     </row>
-    <row r="38" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>44700.697878969906</v>
       </c>
@@ -6262,8 +6520,11 @@
       <c r="AJ38" s="2" t="s">
         <v>118</v>
       </c>
+      <c r="AK38" s="2" t="s">
+        <v>603</v>
+      </c>
     </row>
-    <row r="39" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>44700.701472361106</v>
       </c>
@@ -6372,8 +6633,14 @@
       <c r="AJ39" s="2" t="s">
         <v>120</v>
       </c>
+      <c r="AK39" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="AL39" s="2" t="s">
+        <v>606</v>
+      </c>
     </row>
-    <row r="40" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>44700.708475381944</v>
       </c>
@@ -6479,11 +6746,11 @@
       <c r="AI40" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AJ40" s="2" t="s">
+      <c r="AJ40" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>44700.708819583335</v>
       </c>
@@ -6589,11 +6856,12 @@
       <c r="AI41" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AJ41" s="2" t="s">
+      <c r="AJ41" s="4" t="s">
         <v>124</v>
       </c>
+      <c r="AK41" s="2"/>
     </row>
-    <row r="42" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>44700.710800659726</v>
       </c>
@@ -6702,8 +6970,11 @@
       <c r="AJ42" s="2" t="s">
         <v>126</v>
       </c>
+      <c r="AK42" s="2" t="s">
+        <v>607</v>
+      </c>
     </row>
-    <row r="43" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>44700.711976967592</v>
       </c>
@@ -6812,8 +7083,11 @@
       <c r="AJ43" s="2" t="s">
         <v>128</v>
       </c>
+      <c r="AK43" s="2" t="s">
+        <v>598</v>
+      </c>
     </row>
-    <row r="44" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>44700.715281944445</v>
       </c>
@@ -6922,8 +7196,14 @@
       <c r="AJ44" s="2" t="s">
         <v>130</v>
       </c>
+      <c r="AK44" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="AL44" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="45" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44700.732093530096</v>
       </c>
@@ -7032,8 +7312,11 @@
       <c r="AJ45" s="2" t="s">
         <v>132</v>
       </c>
+      <c r="AK45" s="2" t="s">
+        <v>599</v>
+      </c>
     </row>
-    <row r="46" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>44700.772572118054</v>
       </c>
@@ -7142,8 +7425,11 @@
       <c r="AJ46" s="2" t="s">
         <v>134</v>
       </c>
+      <c r="AK46" s="2" t="s">
+        <v>592</v>
+      </c>
     </row>
-    <row r="47" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>44700.814044155093</v>
       </c>
@@ -7252,8 +7538,11 @@
       <c r="AJ47" s="2" t="s">
         <v>136</v>
       </c>
+      <c r="AK47" s="2" t="s">
+        <v>607</v>
+      </c>
     </row>
-    <row r="48" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>44701.344714050923</v>
       </c>
@@ -7362,8 +7651,11 @@
       <c r="AJ48" s="2" t="s">
         <v>138</v>
       </c>
+      <c r="AK48" s="2" t="s">
+        <v>609</v>
+      </c>
     </row>
-    <row r="49" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>44701.356835497689</v>
       </c>
@@ -7472,8 +7764,14 @@
       <c r="AJ49" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="AK49" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="AM49" s="2" t="s">
+        <v>611</v>
+      </c>
     </row>
-    <row r="50" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>44701.366344988426</v>
       </c>
@@ -7582,8 +7880,14 @@
       <c r="AJ50" s="2" t="s">
         <v>142</v>
       </c>
+      <c r="AK50" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="AL50" s="2" t="s">
+        <v>600</v>
+      </c>
     </row>
-    <row r="51" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>44701.395531956019</v>
       </c>
@@ -7689,11 +7993,12 @@
       <c r="AI51" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="AJ51" s="2" t="s">
+      <c r="AJ51" s="4" t="s">
         <v>144</v>
       </c>
+      <c r="AK51" s="2"/>
     </row>
-    <row r="52" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>44701.396044004628</v>
       </c>
@@ -7802,8 +8107,14 @@
       <c r="AJ52" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="AK52" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="AM52" s="2" t="s">
+        <v>611</v>
+      </c>
     </row>
-    <row r="53" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>44701.400723125</v>
       </c>
@@ -7909,11 +8220,11 @@
       <c r="AI53" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="AJ53" s="2" t="s">
+      <c r="AJ53" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>44701.4010647338</v>
       </c>
@@ -8019,11 +8330,12 @@
       <c r="AI54" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AJ54" s="2" t="s">
+      <c r="AJ54" s="4" t="s">
         <v>150</v>
       </c>
+      <c r="AK54" s="2"/>
     </row>
-    <row r="55" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>44701.41094681713</v>
       </c>
@@ -8129,11 +8441,11 @@
       <c r="AI55" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="AJ55" s="2" t="s">
+      <c r="AJ55" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="56" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>44701.426123819445</v>
       </c>
@@ -8242,8 +8554,14 @@
       <c r="AJ56" s="2" t="s">
         <v>154</v>
       </c>
+      <c r="AK56" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="AM56" s="2" t="s">
+        <v>611</v>
+      </c>
     </row>
-    <row r="57" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>44701.434696469907</v>
       </c>
@@ -8349,11 +8667,11 @@
       <c r="AI57" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="AJ57" s="2" t="s">
+      <c r="AJ57" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="58" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>44701.43636334491</v>
       </c>
@@ -8462,8 +8780,11 @@
       <c r="AJ58" s="2" t="s">
         <v>158</v>
       </c>
+      <c r="AK58" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="59" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>44701.441773506944</v>
       </c>
@@ -8572,8 +8893,14 @@
       <c r="AJ59" s="2" t="s">
         <v>160</v>
       </c>
+      <c r="AK59" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="AL59" s="2" t="s">
+        <v>612</v>
+      </c>
     </row>
-    <row r="60" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>44701.442123958332</v>
       </c>
@@ -8682,8 +9009,17 @@
       <c r="AJ60" s="2" t="s">
         <v>162</v>
       </c>
+      <c r="AK60" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="AL60" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="AM60" s="2" t="s">
+        <v>592</v>
+      </c>
     </row>
-    <row r="61" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>44701.44757822917</v>
       </c>
@@ -8792,8 +9128,11 @@
       <c r="AJ61" s="2" t="s">
         <v>164</v>
       </c>
+      <c r="AK61" s="2" t="s">
+        <v>597</v>
+      </c>
     </row>
-    <row r="62" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>44701.449199502313</v>
       </c>
@@ -8902,8 +9241,11 @@
       <c r="AJ62" s="2" t="s">
         <v>166</v>
       </c>
+      <c r="AK62" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="63" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>44701.457350543977</v>
       </c>
@@ -9012,8 +9354,11 @@
       <c r="AJ63" s="2" t="s">
         <v>168</v>
       </c>
+      <c r="AK63" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="64" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>44701.460796099534</v>
       </c>
@@ -9119,11 +9464,12 @@
       <c r="AI64" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="AJ64" s="2" t="s">
+      <c r="AJ64" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="AK64" s="2"/>
     </row>
-    <row r="65" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>44701.461641875001</v>
       </c>
@@ -9232,8 +9578,14 @@
       <c r="AJ65" s="2" t="s">
         <v>172</v>
       </c>
+      <c r="AK65" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AL65" s="2" t="s">
+        <v>601</v>
+      </c>
     </row>
-    <row r="66" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>44701.46377534722</v>
       </c>
@@ -9342,8 +9694,11 @@
       <c r="AJ66" s="2" t="s">
         <v>174</v>
       </c>
+      <c r="AK66" s="2" t="s">
+        <v>597</v>
+      </c>
     </row>
-    <row r="67" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>44701.468576168976</v>
       </c>
@@ -9452,8 +9807,11 @@
       <c r="AJ67" s="2" t="s">
         <v>176</v>
       </c>
+      <c r="AK67" s="2" t="s">
+        <v>604</v>
+      </c>
     </row>
-    <row r="68" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>44701.471025358798</v>
       </c>
@@ -9562,8 +9920,11 @@
       <c r="AJ68" s="2" t="s">
         <v>178</v>
       </c>
+      <c r="AK68" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="69" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>44701.492433194449</v>
       </c>
@@ -9672,8 +10033,11 @@
       <c r="AJ69" s="2" t="s">
         <v>180</v>
       </c>
+      <c r="AK69" s="2" t="s">
+        <v>609</v>
+      </c>
     </row>
-    <row r="70" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>44701.538276307867</v>
       </c>
@@ -9779,11 +10143,12 @@
       <c r="AI70" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="AJ70" s="2" t="s">
+      <c r="AJ70" s="4" t="s">
         <v>182</v>
       </c>
+      <c r="AK70" s="2"/>
     </row>
-    <row r="71" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>44701.579220983796</v>
       </c>
@@ -9892,8 +10257,11 @@
       <c r="AJ71" s="2" t="s">
         <v>184</v>
       </c>
+      <c r="AK71" s="2" t="s">
+        <v>603</v>
+      </c>
     </row>
-    <row r="72" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>44701.617478356478</v>
       </c>
@@ -10002,8 +10370,11 @@
       <c r="AJ72" s="2" t="s">
         <v>186</v>
       </c>
+      <c r="AK72" s="2" t="s">
+        <v>609</v>
+      </c>
     </row>
-    <row r="73" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>44702.734552789349</v>
       </c>
@@ -10112,8 +10483,14 @@
       <c r="AJ73" s="2" t="s">
         <v>188</v>
       </c>
+      <c r="AK73" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="AL73" s="2" t="s">
+        <v>613</v>
+      </c>
     </row>
-    <row r="74" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>44702.909988425927</v>
       </c>
@@ -10222,8 +10599,14 @@
       <c r="AJ74" s="2" t="s">
         <v>190</v>
       </c>
+      <c r="AK74" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="AL74" s="2" t="s">
+        <v>600</v>
+      </c>
     </row>
-    <row r="75" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>44704.34222071759</v>
       </c>
@@ -10329,11 +10712,11 @@
       <c r="AI75" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="AJ75" s="2">
+      <c r="AJ75" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>44704.405584236112</v>
       </c>
@@ -10439,11 +10822,12 @@
       <c r="AI76" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="AJ76" s="2" t="s">
+      <c r="AJ76" s="4" t="s">
         <v>193</v>
       </c>
+      <c r="AK76" s="2"/>
     </row>
-    <row r="77" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>44704.874857812501</v>
       </c>
@@ -10552,8 +10936,11 @@
       <c r="AJ77" s="2" t="s">
         <v>195</v>
       </c>
+      <c r="AK77" s="2" t="s">
+        <v>614</v>
+      </c>
     </row>
-    <row r="78" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>44706.357278935189</v>
       </c>
@@ -10662,8 +11049,11 @@
       <c r="AJ78" s="2" t="s">
         <v>197</v>
       </c>
+      <c r="AK78" s="2" t="s">
+        <v>615</v>
+      </c>
     </row>
-    <row r="79" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>44706.58037059028</v>
       </c>
@@ -10769,11 +11159,11 @@
       <c r="AI79" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="AJ79" s="2" t="s">
+      <c r="AJ79" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="80" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>44707.466296250001</v>
       </c>
@@ -10882,8 +11272,11 @@
       <c r="AJ80" s="2" t="s">
         <v>201</v>
       </c>
+      <c r="AK80" s="2" t="s">
+        <v>606</v>
+      </c>
     </row>
-    <row r="81" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>44707.490128229168</v>
       </c>
@@ -10992,8 +11385,11 @@
       <c r="AJ81" s="2" t="s">
         <v>203</v>
       </c>
+      <c r="AK81" s="2" t="s">
+        <v>614</v>
+      </c>
     </row>
-    <row r="82" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>44707.506753622685</v>
       </c>
@@ -11102,8 +11498,11 @@
       <c r="AJ82" s="2" t="s">
         <v>205</v>
       </c>
+      <c r="AK82" s="2" t="s">
+        <v>616</v>
+      </c>
     </row>
-    <row r="83" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>44707.539505972221</v>
       </c>
@@ -11212,8 +11611,11 @@
       <c r="AJ83" s="2" t="s">
         <v>207</v>
       </c>
+      <c r="AK83" s="2" t="s">
+        <v>591</v>
+      </c>
     </row>
-    <row r="84" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>44708.419029270837</v>
       </c>
@@ -11319,11 +11721,12 @@
       <c r="AI84" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="AJ84" s="2" t="s">
+      <c r="AJ84" s="4" t="s">
         <v>209</v>
       </c>
+      <c r="AK84" s="2"/>
     </row>
-    <row r="85" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>44708.486562106482</v>
       </c>
@@ -11429,11 +11832,12 @@
       <c r="AI85" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="AJ85" s="2" t="s">
+      <c r="AJ85" s="4" t="s">
         <v>211</v>
       </c>
+      <c r="AK85" s="2"/>
     </row>
-    <row r="86" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>44708.487936759258</v>
       </c>
@@ -11539,11 +11943,11 @@
       <c r="AI86" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="AJ86" s="2" t="s">
+      <c r="AJ86" s="4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="87" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>44708.500332129624</v>
       </c>
@@ -11652,8 +12056,11 @@
       <c r="AJ87" s="2" t="s">
         <v>215</v>
       </c>
+      <c r="AK87" s="2" t="s">
+        <v>592</v>
+      </c>
     </row>
-    <row r="88" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>44708.506765879632</v>
       </c>
@@ -11762,8 +12169,11 @@
       <c r="AJ88" s="2" t="s">
         <v>217</v>
       </c>
+      <c r="AK88" s="2" t="s">
+        <v>603</v>
+      </c>
     </row>
-    <row r="89" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>44708.508628587966</v>
       </c>
@@ -11869,11 +12279,11 @@
       <c r="AI89" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="AJ89" s="2" t="s">
+      <c r="AJ89" s="4" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="90" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>44708.511701504627</v>
       </c>
@@ -11982,8 +12392,11 @@
       <c r="AJ90" s="2" t="s">
         <v>221</v>
       </c>
+      <c r="AK90" s="2" t="s">
+        <v>603</v>
+      </c>
     </row>
-    <row r="91" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>44708.512465266205</v>
       </c>
@@ -12089,11 +12502,11 @@
       <c r="AI91" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="AJ91" s="2" t="s">
+      <c r="AJ91" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="92" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>44708.513208692129</v>
       </c>
@@ -12199,11 +12612,11 @@
       <c r="AI92" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="AJ92" s="2" t="s">
+      <c r="AJ92" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="93" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>44708.514357037042</v>
       </c>
@@ -12312,8 +12725,11 @@
       <c r="AJ93" s="2" t="s">
         <v>226</v>
       </c>
+      <c r="AK93" s="2" t="s">
+        <v>590</v>
+      </c>
     </row>
-    <row r="94" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>44708.518615578709</v>
       </c>
@@ -12419,11 +12835,12 @@
       <c r="AI94" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="AJ94" s="2" t="s">
+      <c r="AJ94" s="4" t="s">
         <v>228</v>
       </c>
+      <c r="AK94" s="2"/>
     </row>
-    <row r="95" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>44708.519329895833</v>
       </c>
@@ -12532,8 +12949,11 @@
       <c r="AJ95" s="2" t="s">
         <v>230</v>
       </c>
+      <c r="AK95" s="2" t="s">
+        <v>599</v>
+      </c>
     </row>
-    <row r="96" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>44708.529904270836</v>
       </c>
@@ -12639,11 +13059,12 @@
       <c r="AI96" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="AJ96" s="2" t="s">
+      <c r="AJ96" s="4" t="s">
         <v>232</v>
       </c>
+      <c r="AK96" s="2"/>
     </row>
-    <row r="97" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>44708.533292743057</v>
       </c>
@@ -12752,8 +13173,11 @@
       <c r="AJ97" s="2" t="s">
         <v>234</v>
       </c>
+      <c r="AK97" s="2" t="s">
+        <v>590</v>
+      </c>
     </row>
-    <row r="98" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>44708.547703090277</v>
       </c>
@@ -12862,8 +13286,11 @@
       <c r="AJ98" s="2" t="s">
         <v>236</v>
       </c>
+      <c r="AK98" s="2" t="s">
+        <v>614</v>
+      </c>
     </row>
-    <row r="99" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>44708.555035266203</v>
       </c>
@@ -12969,11 +13396,11 @@
       <c r="AI99" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="AJ99" s="2" t="s">
+      <c r="AJ99" s="4" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="100" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>44708.617116562498</v>
       </c>
@@ -13079,11 +13506,11 @@
       <c r="AI100" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="AJ100" s="2" t="s">
+      <c r="AJ100" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="101" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>44708.627931180556</v>
       </c>
@@ -13192,8 +13619,11 @@
       <c r="AJ101" s="2" t="s">
         <v>241</v>
       </c>
+      <c r="AK101" s="2" t="s">
+        <v>592</v>
+      </c>
     </row>
-    <row r="102" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>44708.630977662033</v>
       </c>
@@ -13299,11 +13729,11 @@
       <c r="AI102" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="AJ102" s="2" t="s">
+      <c r="AJ102" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="103" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>44708.635544074074</v>
       </c>
@@ -13409,11 +13839,11 @@
       <c r="AI103" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="AJ103" s="2" t="s">
+      <c r="AJ103" s="4" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="104" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>44708.644381365739</v>
       </c>
@@ -13522,8 +13952,11 @@
       <c r="AJ104" s="2" t="s">
         <v>246</v>
       </c>
+      <c r="AK104" s="2" t="s">
+        <v>592</v>
+      </c>
     </row>
-    <row r="105" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>44708.694264768521</v>
       </c>
@@ -13632,8 +14065,11 @@
       <c r="AJ105" s="2" t="s">
         <v>248</v>
       </c>
+      <c r="AK105" s="2" t="s">
+        <v>617</v>
+      </c>
     </row>
-    <row r="106" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>44708.702465289352</v>
       </c>
@@ -13739,11 +14175,11 @@
       <c r="AI106" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="AJ106" s="2" t="s">
+      <c r="AJ106" s="4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="107" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>44708.806698425928</v>
       </c>
@@ -13852,8 +14288,11 @@
       <c r="AJ107" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="AK107" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="108" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>44708.860874143516</v>
       </c>
@@ -13962,8 +14401,14 @@
       <c r="AJ108" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="AK108" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AL108" s="2" t="s">
+        <v>616</v>
+      </c>
     </row>
-    <row r="109" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>44709.05003633102</v>
       </c>
@@ -14069,11 +14514,11 @@
       <c r="AI109" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="AJ109" s="2" t="s">
+      <c r="AJ109" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="110" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>44709.218011851852</v>
       </c>
@@ -14179,11 +14624,11 @@
       <c r="AI110" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="AJ110" s="2" t="s">
+      <c r="AJ110" s="4" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="111" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>44710.191352962967</v>
       </c>
@@ -14289,11 +14734,12 @@
       <c r="AI111" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="AJ111" s="2" t="s">
+      <c r="AJ111" s="4" t="s">
         <v>260</v>
       </c>
+      <c r="AK111" s="2"/>
     </row>
-    <row r="112" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>44710.372184363427</v>
       </c>
@@ -14399,11 +14845,11 @@
       <c r="AI112" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="AJ112" s="2" t="s">
+      <c r="AJ112" s="4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="113" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>44710.389544652775</v>
       </c>
@@ -14512,8 +14958,11 @@
       <c r="AJ113" s="2" t="s">
         <v>264</v>
       </c>
+      <c r="AK113" s="2" t="s">
+        <v>600</v>
+      </c>
     </row>
-    <row r="114" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>44710.444645694442</v>
       </c>
@@ -14622,8 +15071,11 @@
       <c r="AJ114" s="2" t="s">
         <v>266</v>
       </c>
+      <c r="AK114" s="2" t="s">
+        <v>618</v>
+      </c>
     </row>
-    <row r="115" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>44710.686924155088</v>
       </c>
@@ -14729,11 +15181,11 @@
       <c r="AI115" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="AJ115" s="2" t="s">
+      <c r="AJ115" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="116" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>44710.701367685186</v>
       </c>
@@ -14839,11 +15291,11 @@
       <c r="AI116" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="AJ116" s="2" t="s">
+      <c r="AJ116" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="117" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>44710.731109953704</v>
       </c>
@@ -14952,8 +15404,11 @@
       <c r="AJ117" s="2" t="s">
         <v>271</v>
       </c>
+      <c r="AK117" s="2" t="s">
+        <v>619</v>
+      </c>
     </row>
-    <row r="118" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>44710.970941319443</v>
       </c>
@@ -15059,11 +15514,11 @@
       <c r="AI118" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="AJ118" s="2" t="s">
+      <c r="AJ118" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="119" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>44710.9776255787</v>
       </c>
@@ -15172,8 +15627,11 @@
       <c r="AJ119" s="2" t="s">
         <v>274</v>
       </c>
+      <c r="AK119" s="2" t="s">
+        <v>617</v>
+      </c>
     </row>
-    <row r="120" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="3">
         <v>44711.296668831019</v>
       </c>
@@ -15282,8 +15740,11 @@
       <c r="AJ120" s="2" t="s">
         <v>276</v>
       </c>
+      <c r="AK120" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="121" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="3">
         <v>44711.303678553246</v>
       </c>
@@ -15389,11 +15850,11 @@
       <c r="AI121" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="AJ121" s="2" t="s">
+      <c r="AJ121" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="122" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="3">
         <v>44711.324167754632</v>
       </c>
@@ -15499,11 +15960,12 @@
       <c r="AI122" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="AJ122" s="2" t="s">
+      <c r="AJ122" s="4" t="s">
         <v>279</v>
       </c>
+      <c r="AK122" s="2"/>
     </row>
-    <row r="123" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="3">
         <v>44711.333724189812</v>
       </c>
@@ -15612,8 +16074,11 @@
       <c r="AJ123" s="2" t="s">
         <v>281</v>
       </c>
+      <c r="AK123" s="2" t="s">
+        <v>599</v>
+      </c>
     </row>
-    <row r="124" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="3">
         <v>44711.335453865744</v>
       </c>
@@ -15722,8 +16187,11 @@
       <c r="AJ124" s="2" t="s">
         <v>283</v>
       </c>
+      <c r="AK124" s="2" t="s">
+        <v>620</v>
+      </c>
     </row>
-    <row r="125" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="3">
         <v>44711.345245914352</v>
       </c>
@@ -15829,11 +16297,11 @@
       <c r="AI125" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="AJ125" s="2" t="s">
+      <c r="AJ125" s="4" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="126" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="3">
         <v>44711.353050451391</v>
       </c>
@@ -15939,11 +16407,11 @@
       <c r="AI126" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="AJ126" s="2" t="s">
+      <c r="AJ126" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="127" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="3">
         <v>44711.353645567127</v>
       </c>
@@ -16052,8 +16520,11 @@
       <c r="AJ127" s="2" t="s">
         <v>288</v>
       </c>
+      <c r="AK127" s="2" t="s">
+        <v>603</v>
+      </c>
     </row>
-    <row r="128" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="3">
         <v>44711.353935833336</v>
       </c>
@@ -16162,8 +16633,11 @@
       <c r="AJ128" s="2" t="s">
         <v>290</v>
       </c>
+      <c r="AK128" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="129" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="3">
         <v>44711.373942511578</v>
       </c>
@@ -16272,8 +16746,11 @@
       <c r="AJ129" s="2" t="s">
         <v>292</v>
       </c>
+      <c r="AK129" s="2" t="s">
+        <v>597</v>
+      </c>
     </row>
-    <row r="130" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="3">
         <v>44711.392182731477</v>
       </c>
@@ -16379,11 +16856,11 @@
       <c r="AI130" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="AJ130" s="2" t="s">
+      <c r="AJ130" s="4" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="131" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="3">
         <v>44711.396906898153</v>
       </c>
@@ -16489,11 +16966,14 @@
       <c r="AI131" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="AJ131" s="2" t="s">
+      <c r="AJ131" s="4" t="s">
         <v>295</v>
       </c>
+      <c r="AK131" s="2" t="s">
+        <v>629</v>
+      </c>
     </row>
-    <row r="132" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="3">
         <v>44711.413543622686</v>
       </c>
@@ -16599,11 +17079,11 @@
       <c r="AI132" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="AJ132" s="2" t="s">
+      <c r="AJ132" s="4" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="133" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="3">
         <v>44711.422751388891</v>
       </c>
@@ -16709,11 +17189,11 @@
       <c r="AI133" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="AJ133" s="2" t="s">
+      <c r="AJ133" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="134" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="3">
         <v>44711.432632650467</v>
       </c>
@@ -16819,11 +17299,11 @@
       <c r="AI134" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="AJ134" s="2" t="s">
+      <c r="AJ134" s="4" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="135" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="3">
         <v>44711.461834560185</v>
       </c>
@@ -16932,8 +17412,11 @@
       <c r="AJ135" s="2" t="s">
         <v>302</v>
       </c>
+      <c r="AK135" s="2" t="s">
+        <v>603</v>
+      </c>
     </row>
-    <row r="136" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="3">
         <v>44711.483145694445</v>
       </c>
@@ -17042,8 +17525,11 @@
       <c r="AJ136" s="2" t="s">
         <v>304</v>
       </c>
+      <c r="AK136" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="137" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="3">
         <v>44711.483345601853</v>
       </c>
@@ -17152,8 +17638,11 @@
       <c r="AJ137" s="2" t="s">
         <v>305</v>
       </c>
+      <c r="AK137" s="2" t="s">
+        <v>590</v>
+      </c>
     </row>
-    <row r="138" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A138" s="3">
         <v>44711.49073795139</v>
       </c>
@@ -17259,11 +17748,12 @@
       <c r="AI138" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="AJ138" s="2" t="s">
+      <c r="AJ138" s="4" t="s">
         <v>307</v>
       </c>
+      <c r="AK138" s="2"/>
     </row>
-    <row r="139" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="3">
         <v>44711.496015381941</v>
       </c>
@@ -17369,11 +17859,11 @@
       <c r="AI139" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="AJ139" s="2" t="s">
+      <c r="AJ139" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="140" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="3">
         <v>44711.569164212968</v>
       </c>
@@ -17482,8 +17972,11 @@
       <c r="AJ140" s="2" t="s">
         <v>310</v>
       </c>
+      <c r="AK140" s="2" t="s">
+        <v>606</v>
+      </c>
     </row>
-    <row r="141" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A141" s="3">
         <v>44711.576844409719</v>
       </c>
@@ -17592,8 +18085,11 @@
       <c r="AJ141" s="2" t="s">
         <v>312</v>
       </c>
+      <c r="AK141" s="2" t="s">
+        <v>621</v>
+      </c>
     </row>
-    <row r="142" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="3">
         <v>44711.583180856484</v>
       </c>
@@ -17699,11 +18195,14 @@
       <c r="AI142" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="AJ142" s="2" t="s">
+      <c r="AJ142" s="4" t="s">
         <v>314</v>
       </c>
+      <c r="AK142" s="5" t="s">
+        <v>591</v>
+      </c>
     </row>
-    <row r="143" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="3">
         <v>44711.594780995365</v>
       </c>
@@ -17809,11 +18308,11 @@
       <c r="AI143" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="AJ143" s="2" t="s">
+      <c r="AJ143" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="144" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="3">
         <v>44711.598220810185</v>
       </c>
@@ -17919,11 +18418,11 @@
       <c r="AI144" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="AJ144" s="2" t="s">
+      <c r="AJ144" s="4" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="145" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="3">
         <v>44711.619002268519</v>
       </c>
@@ -18029,11 +18528,11 @@
       <c r="AI145" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="AJ145" s="2" t="s">
+      <c r="AJ145" s="4" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="146" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="3">
         <v>44711.633848831014</v>
       </c>
@@ -18139,11 +18638,12 @@
       <c r="AI146" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="AJ146" s="2" t="s">
+      <c r="AJ146" s="4" t="s">
         <v>321</v>
       </c>
+      <c r="AK146" s="2"/>
     </row>
-    <row r="147" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="3">
         <v>44711.709409664356</v>
       </c>
@@ -18252,8 +18752,14 @@
       <c r="AJ147" s="2" t="s">
         <v>323</v>
       </c>
+      <c r="AK147" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="AL147" s="2" t="s">
+        <v>601</v>
+      </c>
     </row>
-    <row r="148" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="3">
         <v>44712.298463425926</v>
       </c>
@@ -18359,11 +18865,11 @@
       <c r="AI148" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="AJ148" s="2" t="s">
+      <c r="AJ148" s="4" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="149" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" s="3">
         <v>44712.344813796299</v>
       </c>
@@ -18469,11 +18975,11 @@
       <c r="AI149" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="AJ149" s="2" t="s">
+      <c r="AJ149" s="4" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="150" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="3">
         <v>44712.349009027777</v>
       </c>
@@ -18582,8 +19088,11 @@
       <c r="AJ150" s="2" t="s">
         <v>329</v>
       </c>
+      <c r="AK150" s="2" t="s">
+        <v>621</v>
+      </c>
     </row>
-    <row r="151" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="3">
         <v>44712.550696724538</v>
       </c>
@@ -18689,11 +19198,11 @@
       <c r="AI151" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="AJ151" s="4" t="s">
+      <c r="AJ151" s="6" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="152" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="3">
         <v>44712.563506701394</v>
       </c>
@@ -18799,11 +19308,11 @@
       <c r="AI152" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="AJ152" s="2" t="s">
+      <c r="AJ152" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="153" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="3">
         <v>44712.569732581018</v>
       </c>
@@ -18912,8 +19421,11 @@
       <c r="AJ153" s="2" t="s">
         <v>334</v>
       </c>
+      <c r="AK153" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="154" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A154" s="3">
         <v>44712.670201458328</v>
       </c>
@@ -19022,8 +19534,14 @@
       <c r="AJ154" s="2" t="s">
         <v>336</v>
       </c>
+      <c r="AK154" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="AL154" s="2" t="s">
+        <v>623</v>
+      </c>
     </row>
-    <row r="155" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A155" s="3">
         <v>44712.670746643518</v>
       </c>
@@ -19132,8 +19650,11 @@
       <c r="AJ155" s="2" t="s">
         <v>338</v>
       </c>
+      <c r="AK155" s="2" t="s">
+        <v>592</v>
+      </c>
     </row>
-    <row r="156" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="3">
         <v>44712.701295752311</v>
       </c>
@@ -19239,11 +19760,11 @@
       <c r="AI156" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="AJ156" s="2" t="s">
+      <c r="AJ156" s="4" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="157" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A157" s="3">
         <v>44712.722038784719</v>
       </c>
@@ -19352,8 +19873,11 @@
       <c r="AJ157" s="2" t="s">
         <v>342</v>
       </c>
+      <c r="AK157" s="2" t="s">
+        <v>621</v>
+      </c>
     </row>
-    <row r="158" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A158" s="3">
         <v>44712.786999594908</v>
       </c>
@@ -19459,11 +19983,11 @@
       <c r="AI158" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="AJ158" s="2" t="s">
+      <c r="AJ158" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="159" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" s="3">
         <v>44713.218581319445</v>
       </c>
@@ -19569,11 +20093,11 @@
       <c r="AI159" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="AJ159" s="2" t="s">
+      <c r="AJ159" s="4" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="160" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" s="3">
         <v>44713.21926341435</v>
       </c>
@@ -19679,11 +20203,12 @@
       <c r="AI160" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="AJ160" s="2" t="s">
+      <c r="AJ160" s="4" t="s">
         <v>346</v>
       </c>
+      <c r="AK160" s="2"/>
     </row>
-    <row r="161" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" s="3">
         <v>44713.296575231478</v>
       </c>
@@ -19792,8 +20317,11 @@
       <c r="AJ161" s="2" t="s">
         <v>348</v>
       </c>
+      <c r="AK161" s="2" t="s">
+        <v>599</v>
+      </c>
     </row>
-    <row r="162" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A162" s="3">
         <v>44713.38194663194</v>
       </c>
@@ -19902,8 +20430,11 @@
       <c r="AJ162" s="2" t="s">
         <v>350</v>
       </c>
+      <c r="AK162" s="2" t="s">
+        <v>616</v>
+      </c>
     </row>
-    <row r="163" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" s="3">
         <v>44713.449858472217</v>
       </c>
@@ -20012,8 +20543,11 @@
       <c r="AJ163" s="2" t="s">
         <v>352</v>
       </c>
+      <c r="AK163" s="2" t="s">
+        <v>603</v>
+      </c>
     </row>
-    <row r="164" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A164" s="3">
         <v>44713.474393414348</v>
       </c>
@@ -20119,11 +20653,12 @@
       <c r="AI164" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="AJ164" s="2" t="s">
+      <c r="AJ164" s="4" t="s">
         <v>354</v>
       </c>
+      <c r="AK164" s="2"/>
     </row>
-    <row r="165" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A165" s="3">
         <v>44713.519721620367</v>
       </c>
@@ -20232,8 +20767,11 @@
       <c r="AJ165" s="2" t="s">
         <v>356</v>
       </c>
+      <c r="AK165" s="2" t="s">
+        <v>606</v>
+      </c>
     </row>
-    <row r="166" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A166" s="3">
         <v>44713.537470069445</v>
       </c>
@@ -20339,11 +20877,12 @@
       <c r="AI166" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="AJ166" s="2" t="s">
+      <c r="AJ166" s="4" t="s">
         <v>358</v>
       </c>
+      <c r="AK166" s="2"/>
     </row>
-    <row r="167" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A167" s="3">
         <v>44713.626116493055</v>
       </c>
@@ -20452,8 +20991,11 @@
       <c r="AJ167" s="2" t="s">
         <v>360</v>
       </c>
+      <c r="AK167" s="2" t="s">
+        <v>591</v>
+      </c>
     </row>
-    <row r="168" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A168" s="3">
         <v>44713.963422500005</v>
       </c>
@@ -20562,8 +21104,11 @@
       <c r="AJ168" s="2" t="s">
         <v>362</v>
       </c>
+      <c r="AK168" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="169" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A169" s="3">
         <v>44714.033295752313</v>
       </c>
@@ -20669,11 +21214,12 @@
       <c r="AI169" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="AJ169" s="2" t="s">
+      <c r="AJ169" s="4" t="s">
         <v>364</v>
       </c>
+      <c r="AK169" s="2"/>
     </row>
-    <row r="170" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A170" s="3">
         <v>44714.340098263885</v>
       </c>
@@ -20782,8 +21328,11 @@
       <c r="AJ170" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="AK170" s="2" t="s">
+        <v>603</v>
+      </c>
     </row>
-    <row r="171" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A171" s="3">
         <v>44714.351784618055</v>
       </c>
@@ -20889,11 +21438,11 @@
       <c r="AI171" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="AJ171" s="2" t="s">
+      <c r="AJ171" s="4" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="172" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A172" s="3">
         <v>44714.360026006943</v>
       </c>
@@ -20999,11 +21548,11 @@
       <c r="AI172" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="AJ172" s="2" t="s">
+      <c r="AJ172" s="4" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="173" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A173" s="3">
         <v>44714.37194118055</v>
       </c>
@@ -21109,11 +21658,11 @@
       <c r="AI173" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="AJ173" s="2" t="s">
+      <c r="AJ173" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="174" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A174" s="3">
         <v>44714.396471030093</v>
       </c>
@@ -21219,11 +21768,11 @@
       <c r="AI174" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="AJ174" s="2" t="s">
+      <c r="AJ174" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="175" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A175" s="3">
         <v>44714.398405856482</v>
       </c>
@@ -21332,8 +21881,11 @@
       <c r="AJ175" s="2" t="s">
         <v>374</v>
       </c>
+      <c r="AK175" s="2" t="s">
+        <v>614</v>
+      </c>
     </row>
-    <row r="176" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A176" s="3">
         <v>44714.410918368056</v>
       </c>
@@ -21442,8 +21994,11 @@
       <c r="AJ176" s="2" t="s">
         <v>376</v>
       </c>
+      <c r="AK176" s="2" t="s">
+        <v>597</v>
+      </c>
     </row>
-    <row r="177" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A177" s="3">
         <v>44714.416994918982</v>
       </c>
@@ -21549,11 +22104,11 @@
       <c r="AI177" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="AJ177" s="2" t="s">
+      <c r="AJ177" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="178" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A178" s="3">
         <v>44714.423816099537</v>
       </c>
@@ -21659,11 +22214,11 @@
       <c r="AI178" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="AJ178" s="2" t="s">
+      <c r="AJ178" s="4" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="179" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A179" s="3">
         <v>44714.4345178125</v>
       </c>
@@ -21769,11 +22324,11 @@
       <c r="AI179" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="AJ179" s="2" t="s">
+      <c r="AJ179" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="180" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A180" s="3">
         <v>44714.435199259256</v>
       </c>
@@ -21882,8 +22437,11 @@
       <c r="AJ180" s="2" t="s">
         <v>382</v>
       </c>
+      <c r="AK180" s="2" t="s">
+        <v>600</v>
+      </c>
     </row>
-    <row r="181" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A181" s="3">
         <v>44714.43530730324</v>
       </c>
@@ -21989,11 +22547,12 @@
       <c r="AI181" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="AJ181" s="2" t="s">
+      <c r="AJ181" s="4" t="s">
         <v>384</v>
       </c>
+      <c r="AK181" s="2"/>
     </row>
-    <row r="182" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A182" s="3">
         <v>44714.546710891205</v>
       </c>
@@ -22099,11 +22658,12 @@
       <c r="AI182" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="AJ182" s="2" t="s">
+      <c r="AJ182" s="4" t="s">
         <v>386</v>
       </c>
+      <c r="AK182" s="2"/>
     </row>
-    <row r="183" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A183" s="3">
         <v>44718.364490428241</v>
       </c>
@@ -22209,11 +22769,11 @@
       <c r="AI183" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="AJ183" s="2" t="s">
+      <c r="AJ183" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="184" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A184" s="3">
         <v>44719.673474236115</v>
       </c>
@@ -22322,8 +22882,11 @@
       <c r="AJ184" s="2" t="s">
         <v>389</v>
       </c>
+      <c r="AK184" s="2" t="s">
+        <v>600</v>
+      </c>
     </row>
-    <row r="185" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A185" s="3">
         <v>44719.718846064818</v>
       </c>
@@ -22432,8 +22995,11 @@
       <c r="AJ185" s="2" t="s">
         <v>390</v>
       </c>
+      <c r="AK185" s="2" t="s">
+        <v>597</v>
+      </c>
     </row>
-    <row r="186" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A186" s="3">
         <v>44719.733762638891</v>
       </c>
@@ -22542,8 +23108,14 @@
       <c r="AJ186" s="2" t="s">
         <v>392</v>
       </c>
+      <c r="AK186" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AL186" s="2" t="s">
+        <v>601</v>
+      </c>
     </row>
-    <row r="187" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A187" s="3">
         <v>44720.369135462963</v>
       </c>
@@ -22649,11 +23221,12 @@
       <c r="AI187" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="AJ187" s="2" t="s">
+      <c r="AJ187" s="4" t="s">
         <v>394</v>
       </c>
+      <c r="AK187" s="2"/>
     </row>
-    <row r="188" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A188" s="3">
         <v>44720.369483472226</v>
       </c>
@@ -22762,8 +23335,11 @@
       <c r="AJ188" s="2" t="s">
         <v>396</v>
       </c>
+      <c r="AK188" s="2" t="s">
+        <v>616</v>
+      </c>
     </row>
-    <row r="189" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A189" s="3">
         <v>44720.371962395831</v>
       </c>
@@ -22869,11 +23445,11 @@
       <c r="AI189" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="AJ189" s="2" t="s">
+      <c r="AJ189" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="190" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A190" s="3">
         <v>44720.383613194441</v>
       </c>
@@ -22979,11 +23555,11 @@
       <c r="AI190" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="AJ190" s="2" t="s">
+      <c r="AJ190" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="191" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A191" s="3">
         <v>44720.408109687502</v>
       </c>
@@ -23089,11 +23665,12 @@
       <c r="AI191" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="AJ191" s="2" t="s">
+      <c r="AJ191" s="4" t="s">
         <v>400</v>
       </c>
+      <c r="AK191" s="2"/>
     </row>
-    <row r="192" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A192" s="3">
         <v>44720.420756030093</v>
       </c>
@@ -23202,8 +23779,17 @@
       <c r="AJ192" s="2" t="s">
         <v>402</v>
       </c>
+      <c r="AK192" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AL192" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="AM192" s="2" t="s">
+        <v>603</v>
+      </c>
     </row>
-    <row r="193" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A193" s="3">
         <v>44720.49820667824</v>
       </c>
@@ -23312,8 +23898,14 @@
       <c r="AJ193" s="2" t="s">
         <v>404</v>
       </c>
+      <c r="AK193" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="AL193" s="2" t="s">
+        <v>603</v>
+      </c>
     </row>
-    <row r="194" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A194" s="3">
         <v>44720.519295810183</v>
       </c>
@@ -23422,8 +24014,11 @@
       <c r="AJ194" s="2" t="s">
         <v>406</v>
       </c>
+      <c r="AK194" s="2" t="s">
+        <v>624</v>
+      </c>
     </row>
-    <row r="195" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A195" s="3">
         <v>44720.531257465278</v>
       </c>
@@ -23529,11 +24124,12 @@
       <c r="AI195" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="AJ195" s="2" t="s">
+      <c r="AJ195" s="4" t="s">
         <v>408</v>
       </c>
+      <c r="AK195" s="2"/>
     </row>
-    <row r="196" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A196" s="3">
         <v>44720.564305775464</v>
       </c>
@@ -23642,8 +24238,11 @@
       <c r="AJ196" s="2" t="s">
         <v>410</v>
       </c>
+      <c r="AK196" s="2" t="s">
+        <v>600</v>
+      </c>
     </row>
-    <row r="197" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A197" s="3">
         <v>44720.585429537037</v>
       </c>
@@ -23752,8 +24351,14 @@
       <c r="AJ197" s="2" t="s">
         <v>412</v>
       </c>
+      <c r="AK197" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="AL197" s="2" t="s">
+        <v>625</v>
+      </c>
     </row>
-    <row r="198" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A198" s="3">
         <v>44720.599359131942</v>
       </c>
@@ -23859,11 +24464,12 @@
       <c r="AI198" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="AJ198" s="2" t="s">
+      <c r="AJ198" s="4" t="s">
         <v>414</v>
       </c>
+      <c r="AK198" s="2"/>
     </row>
-    <row r="199" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A199" s="3">
         <v>44720.607525462961</v>
       </c>
@@ -23969,11 +24575,12 @@
       <c r="AI199" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="AJ199" s="2" t="s">
+      <c r="AJ199" s="4" t="s">
         <v>416</v>
       </c>
+      <c r="AK199" s="2"/>
     </row>
-    <row r="200" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A200" s="3">
         <v>44720.61301296296</v>
       </c>
@@ -24079,11 +24686,12 @@
       <c r="AI200" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="AJ200" s="2" t="s">
+      <c r="AJ200" s="4" t="s">
         <v>418</v>
       </c>
+      <c r="AK200" s="2"/>
     </row>
-    <row r="201" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A201" s="3">
         <v>44720.634302453705</v>
       </c>
@@ -24189,11 +24797,11 @@
       <c r="AI201" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="AJ201" s="2" t="s">
+      <c r="AJ201" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="202" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A202" s="3">
         <v>44720.636603946754</v>
       </c>
@@ -24302,8 +24910,11 @@
       <c r="AJ202" s="2" t="s">
         <v>421</v>
       </c>
+      <c r="AK202" s="2" t="s">
+        <v>605</v>
+      </c>
     </row>
-    <row r="203" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A203" s="3">
         <v>44720.649415925931</v>
       </c>
@@ -24409,11 +25020,11 @@
       <c r="AI203" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="AJ203" s="2" t="s">
+      <c r="AJ203" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="204" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A204" s="3">
         <v>44720.656220717588</v>
       </c>
@@ -24522,8 +25133,11 @@
       <c r="AJ204" s="2" t="s">
         <v>424</v>
       </c>
+      <c r="AK204" s="2" t="s">
+        <v>625</v>
+      </c>
     </row>
-    <row r="205" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A205" s="3">
         <v>44720.664524699074</v>
       </c>
@@ -24632,8 +25246,11 @@
       <c r="AJ205" s="2" t="s">
         <v>426</v>
       </c>
+      <c r="AK205" s="2" t="s">
+        <v>592</v>
+      </c>
     </row>
-    <row r="206" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A206" s="3">
         <v>44720.665442962963</v>
       </c>
@@ -24742,8 +25359,11 @@
       <c r="AJ206" s="2" t="s">
         <v>428</v>
       </c>
+      <c r="AK206" s="2" t="s">
+        <v>625</v>
+      </c>
     </row>
-    <row r="207" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A207" s="3">
         <v>44720.677891874999</v>
       </c>
@@ -24849,11 +25469,12 @@
       <c r="AI207" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="AJ207" s="2" t="s">
+      <c r="AJ207" s="4" t="s">
         <v>430</v>
       </c>
+      <c r="AK207" s="2"/>
     </row>
-    <row r="208" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A208" s="3">
         <v>44720.682563900467</v>
       </c>
@@ -24959,11 +25580,11 @@
       <c r="AI208" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="AJ208" s="2" t="s">
+      <c r="AJ208" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="209" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A209" s="3">
         <v>44720.708638171302</v>
       </c>
@@ -25069,11 +25690,12 @@
       <c r="AI209" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="AJ209" s="2" t="s">
+      <c r="AJ209" s="4" t="s">
         <v>433</v>
       </c>
+      <c r="AK209" s="2"/>
     </row>
-    <row r="210" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A210" s="3">
         <v>44720.812811284719</v>
       </c>
@@ -25179,11 +25801,12 @@
       <c r="AI210" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="AJ210" s="2" t="s">
+      <c r="AJ210" s="4" t="s">
         <v>435</v>
       </c>
+      <c r="AK210" s="2"/>
     </row>
-    <row r="211" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A211" s="3">
         <v>44720.840268761574</v>
       </c>
@@ -25289,11 +25912,12 @@
       <c r="AI211" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="AJ211" s="2" t="s">
+      <c r="AJ211" s="4" t="s">
         <v>437</v>
       </c>
+      <c r="AK211" s="2"/>
     </row>
-    <row r="212" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A212" s="3">
         <v>44720.878762696761</v>
       </c>
@@ -25402,8 +26026,11 @@
       <c r="AJ212" s="2" t="s">
         <v>439</v>
       </c>
+      <c r="AK212" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="213" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A213" s="3">
         <v>44721.33600195602</v>
       </c>
@@ -25512,8 +26139,11 @@
       <c r="AJ213" s="2" t="s">
         <v>441</v>
       </c>
+      <c r="AK213" s="2" t="s">
+        <v>618</v>
+      </c>
     </row>
-    <row r="214" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A214" s="3">
         <v>44721.461608136575</v>
       </c>
@@ -25622,8 +26252,11 @@
       <c r="AJ214" s="2" t="s">
         <v>443</v>
       </c>
+      <c r="AK214" s="2" t="s">
+        <v>617</v>
+      </c>
     </row>
-    <row r="215" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A215" s="3">
         <v>44721.49142298611</v>
       </c>
@@ -25732,8 +26365,11 @@
       <c r="AJ215" s="2" t="s">
         <v>445</v>
       </c>
+      <c r="AK215" s="2" t="s">
+        <v>600</v>
+      </c>
     </row>
-    <row r="216" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A216" s="3">
         <v>44721.620303206015</v>
       </c>
@@ -25839,11 +26475,12 @@
       <c r="AI216" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="AJ216" s="2" t="s">
+      <c r="AJ216" s="4" t="s">
         <v>447</v>
       </c>
+      <c r="AK216" s="2"/>
     </row>
-    <row r="217" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A217" s="3">
         <v>44721.667338148152</v>
       </c>
@@ -25952,8 +26589,11 @@
       <c r="AJ217" s="2" t="s">
         <v>449</v>
       </c>
+      <c r="AK217" s="2" t="s">
+        <v>591</v>
+      </c>
     </row>
-    <row r="218" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A218" s="3">
         <v>44721.870988263894</v>
       </c>
@@ -26062,8 +26702,11 @@
       <c r="AJ218" s="2" t="s">
         <v>451</v>
       </c>
+      <c r="AK218" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="219" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A219" s="3">
         <v>44722.318691168985</v>
       </c>
@@ -26169,11 +26812,12 @@
       <c r="AI219" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="AJ219" s="2" t="s">
+      <c r="AJ219" s="4" t="s">
         <v>453</v>
       </c>
+      <c r="AK219" s="2"/>
     </row>
-    <row r="220" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A220" s="3">
         <v>44722.376613587963</v>
       </c>
@@ -26279,11 +26923,11 @@
       <c r="AI220" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="AJ220" s="2" t="s">
+      <c r="AJ220" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="221" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A221" s="3">
         <v>44722.418405347227</v>
       </c>
@@ -26389,11 +27033,11 @@
       <c r="AI221" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="AJ221" s="2" t="s">
+      <c r="AJ221" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="222" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A222" s="3">
         <v>44722.426486087963</v>
       </c>
@@ -26499,11 +27143,11 @@
       <c r="AI222" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="AJ222" s="2" t="s">
+      <c r="AJ222" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="223" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A223" s="3">
         <v>44722.47393670139</v>
       </c>
@@ -26612,8 +27256,11 @@
       <c r="AJ223" s="2" t="s">
         <v>458</v>
       </c>
+      <c r="AK223" s="2" t="s">
+        <v>592</v>
+      </c>
     </row>
-    <row r="224" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A224" s="3">
         <v>44722.826001527777</v>
       </c>
@@ -26722,8 +27369,11 @@
       <c r="AJ224" s="2" t="s">
         <v>460</v>
       </c>
+      <c r="AK224" s="2" t="s">
+        <v>597</v>
+      </c>
     </row>
-    <row r="225" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A225" s="3">
         <v>44723.439682592594</v>
       </c>
@@ -26832,8 +27482,11 @@
       <c r="AJ225" s="2" t="s">
         <v>461</v>
       </c>
+      <c r="AK225" s="2" t="s">
+        <v>592</v>
+      </c>
     </row>
-    <row r="226" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A226" s="3">
         <v>44725.836746805551</v>
       </c>
@@ -26939,11 +27592,12 @@
       <c r="AI226" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="AJ226" s="2" t="s">
+      <c r="AJ226" s="4" t="s">
         <v>463</v>
       </c>
+      <c r="AK226" s="2"/>
     </row>
-    <row r="227" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A227" s="3">
         <v>44728.689555833334</v>
       </c>
@@ -27049,11 +27703,12 @@
       <c r="AI227" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="AJ227" s="2" t="s">
+      <c r="AJ227" s="4" t="s">
         <v>465</v>
       </c>
+      <c r="AK227" s="2"/>
     </row>
-    <row r="228" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A228" s="3">
         <v>44729.484426712967</v>
       </c>
@@ -27159,11 +27814,11 @@
       <c r="AI228" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="AJ228" s="2" t="s">
+      <c r="AJ228" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="229" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A229" s="3">
         <v>44729.506572442129</v>
       </c>
@@ -27272,8 +27927,11 @@
       <c r="AJ229" s="2" t="s">
         <v>468</v>
       </c>
+      <c r="AK229" s="2" t="s">
+        <v>600</v>
+      </c>
     </row>
-    <row r="230" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A230" s="3">
         <v>44734.432389155088</v>
       </c>
@@ -27382,8 +28040,14 @@
       <c r="AJ230" s="2" t="s">
         <v>470</v>
       </c>
+      <c r="AK230" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="AL230" s="2" t="s">
+        <v>603</v>
+      </c>
     </row>
-    <row r="231" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A231" s="3">
         <v>44735.370827962965</v>
       </c>
@@ -27489,11 +28153,11 @@
       <c r="AI231" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="AJ231" s="2" t="s">
+      <c r="AJ231" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="232" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A232" s="3">
         <v>44735.375377627315</v>
       </c>
@@ -27599,11 +28263,11 @@
       <c r="AI232" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="AJ232" s="2" t="s">
+      <c r="AJ232" s="4" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="233" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A233" s="3">
         <v>44735.378988946759</v>
       </c>
@@ -27712,8 +28376,14 @@
       <c r="AJ233" s="2" t="s">
         <v>474</v>
       </c>
+      <c r="AK233" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="AL233" s="2" t="s">
+        <v>600</v>
+      </c>
     </row>
-    <row r="234" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A234" s="3">
         <v>44735.493360416665</v>
       </c>
@@ -27822,8 +28492,11 @@
       <c r="AJ234" s="2" t="s">
         <v>476</v>
       </c>
+      <c r="AK234" s="2" t="s">
+        <v>625</v>
+      </c>
     </row>
-    <row r="235" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A235" s="3">
         <v>44735.613156064814</v>
       </c>
@@ -27932,8 +28605,11 @@
       <c r="AJ235" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="AK235" s="2" t="s">
+        <v>614</v>
+      </c>
     </row>
-    <row r="236" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A236" s="3">
         <v>44735.641460208339</v>
       </c>
@@ -28042,8 +28718,11 @@
       <c r="AJ236" s="2" t="s">
         <v>480</v>
       </c>
+      <c r="AK236" s="2" t="s">
+        <v>590</v>
+      </c>
     </row>
-    <row r="237" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A237" s="3">
         <v>44735.653219270833</v>
       </c>
@@ -28149,11 +28828,12 @@
       <c r="AI237" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="AJ237" s="2" t="s">
+      <c r="AJ237" s="4" t="s">
         <v>482</v>
       </c>
+      <c r="AK237" s="2"/>
     </row>
-    <row r="238" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A238" s="3">
         <v>44735.661782384261</v>
       </c>
@@ -28259,11 +28939,11 @@
       <c r="AI238" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="AJ238" s="2" t="s">
+      <c r="AJ238" s="4" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="239" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A239" s="3">
         <v>44735.682017777777</v>
       </c>
@@ -28372,8 +29052,11 @@
       <c r="AJ239" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="AK239" s="2" t="s">
+        <v>614</v>
+      </c>
     </row>
-    <row r="240" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A240" s="3">
         <v>44735.686047314812</v>
       </c>
@@ -28482,8 +29165,14 @@
       <c r="AJ240" s="2" t="s">
         <v>487</v>
       </c>
+      <c r="AK240" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="AL240" s="2" t="s">
+        <v>606</v>
+      </c>
     </row>
-    <row r="241" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A241" s="3">
         <v>44735.773633888894</v>
       </c>
@@ -28592,8 +29281,14 @@
       <c r="AJ241" s="2" t="s">
         <v>489</v>
       </c>
+      <c r="AK241" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="AL241" s="2" t="s">
+        <v>627</v>
+      </c>
     </row>
-    <row r="242" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A242" s="3">
         <v>44735.842642557865</v>
       </c>
@@ -28699,11 +29394,11 @@
       <c r="AI242" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AJ242" s="2" t="s">
+      <c r="AJ242" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="243" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A243" s="3">
         <v>44735.904051678241</v>
       </c>
@@ -28809,11 +29504,11 @@
       <c r="AI243" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="AJ243" s="2" t="s">
+      <c r="AJ243" s="4" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="244" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A244" s="3">
         <v>44735.996122187498</v>
       </c>
@@ -28919,11 +29614,11 @@
       <c r="AI244" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="AJ244" s="2" t="s">
+      <c r="AJ244" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="245" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A245" s="3">
         <v>44736.341773159722</v>
       </c>
@@ -29032,8 +29727,11 @@
       <c r="AJ245" s="2" t="s">
         <v>494</v>
       </c>
+      <c r="AK245" s="2" t="s">
+        <v>599</v>
+      </c>
     </row>
-    <row r="246" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A246" s="3">
         <v>44736.366380960651</v>
       </c>
@@ -29139,11 +29837,11 @@
       <c r="AI246" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="AJ246" s="2" t="s">
+      <c r="AJ246" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="247" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A247" s="3">
         <v>44736.371140520831</v>
       </c>
@@ -29252,8 +29950,11 @@
       <c r="AJ247" s="2" t="s">
         <v>497</v>
       </c>
+      <c r="AK247" s="2" t="s">
+        <v>614</v>
+      </c>
     </row>
-    <row r="248" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A248" s="3">
         <v>44736.410788472218</v>
       </c>
@@ -29359,11 +30060,12 @@
       <c r="AI248" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="AJ248" s="2" t="s">
+      <c r="AJ248" s="4" t="s">
         <v>499</v>
       </c>
+      <c r="AK248" s="2"/>
     </row>
-    <row r="249" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A249" s="3">
         <v>44736.44506706018</v>
       </c>
@@ -29469,11 +30171,11 @@
       <c r="AI249" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="AJ249" s="2" t="s">
+      <c r="AJ249" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="250" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A250" s="3">
         <v>44736.521205115743</v>
       </c>
@@ -29579,11 +30281,11 @@
       <c r="AI250" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="AJ250" s="2" t="s">
+      <c r="AJ250" s="4" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="251" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A251" s="3">
         <v>44736.561308946759</v>
       </c>
@@ -29692,8 +30394,11 @@
       <c r="AJ251" s="2" t="s">
         <v>504</v>
       </c>
+      <c r="AK251" s="2" t="s">
+        <v>596</v>
+      </c>
     </row>
-    <row r="252" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A252" s="3">
         <v>44736.663646157409</v>
       </c>
@@ -29799,11 +30504,12 @@
       <c r="AI252" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="AJ252" s="2" t="s">
+      <c r="AJ252" s="4" t="s">
         <v>506</v>
       </c>
+      <c r="AK252" s="2"/>
     </row>
-    <row r="253" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A253" s="3">
         <v>44736.714509930556</v>
       </c>
@@ -29909,11 +30615,11 @@
       <c r="AI253" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="AJ253" s="2" t="s">
+      <c r="AJ253" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="254" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A254" s="3">
         <v>44736.734705798612</v>
       </c>
@@ -30019,11 +30725,11 @@
       <c r="AI254" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="AJ254" s="2" t="s">
+      <c r="AJ254" s="4" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="255" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A255" s="3">
         <v>44736.808461979163</v>
       </c>
@@ -30129,11 +30835,12 @@
       <c r="AI255" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="AJ255" s="2" t="s">
+      <c r="AJ255" s="4" t="s">
         <v>511</v>
       </c>
+      <c r="AK255" s="2"/>
     </row>
-    <row r="256" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A256" s="3">
         <v>44736.812763865746</v>
       </c>
@@ -30239,11 +30946,11 @@
       <c r="AI256" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="AJ256" s="2" t="s">
+      <c r="AJ256" s="4" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="257" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A257" s="3">
         <v>44736.815987916663</v>
       </c>
@@ -30349,11 +31056,12 @@
       <c r="AI257" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="AJ257" s="2" t="s">
+      <c r="AJ257" s="4" t="s">
         <v>144</v>
       </c>
+      <c r="AK257" s="2"/>
     </row>
-    <row r="258" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A258" s="3">
         <v>44736.962626099536</v>
       </c>
@@ -30459,11 +31167,12 @@
       <c r="AI258" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="AJ258" s="2" t="s">
+      <c r="AJ258" s="4" t="s">
         <v>144</v>
       </c>
+      <c r="AK258" s="2"/>
     </row>
-    <row r="259" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A259" s="3">
         <v>44736.964375439813</v>
       </c>
@@ -30572,8 +31281,11 @@
       <c r="AJ259" s="2" t="s">
         <v>517</v>
       </c>
+      <c r="AK259" s="2" t="s">
+        <v>617</v>
+      </c>
     </row>
-    <row r="260" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A260" s="3">
         <v>44736.975246192131</v>
       </c>
@@ -30679,11 +31391,11 @@
       <c r="AI260" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AJ260" s="2" t="s">
+      <c r="AJ260" s="4" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="261" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A261" s="3">
         <v>44737.00266805556</v>
       </c>
@@ -30789,11 +31501,11 @@
       <c r="AI261" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="AJ261" s="2" t="s">
+      <c r="AJ261" s="4" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="262" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A262" s="3">
         <v>44737.425198958328</v>
       </c>
@@ -30902,8 +31614,11 @@
       <c r="AJ262" s="2" t="s">
         <v>521</v>
       </c>
+      <c r="AK262" s="2" t="s">
+        <v>618</v>
+      </c>
     </row>
-    <row r="263" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A263" s="3">
         <v>44737.956790914352</v>
       </c>
@@ -31012,8 +31727,11 @@
       <c r="AJ263" s="2" t="s">
         <v>523</v>
       </c>
+      <c r="AK263" s="2" t="s">
+        <v>617</v>
+      </c>
     </row>
-    <row r="264" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A264" s="3">
         <v>44738.051874907411</v>
       </c>
@@ -31119,11 +31837,11 @@
       <c r="AI264" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="AJ264" s="2" t="s">
+      <c r="AJ264" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="265" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A265" s="3">
         <v>44738.05187737268</v>
       </c>
@@ -31229,11 +31947,11 @@
       <c r="AI265" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="AJ265" s="2" t="s">
+      <c r="AJ265" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="266" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A266" s="3">
         <v>44738.630495624995</v>
       </c>
@@ -31342,8 +32060,11 @@
       <c r="AJ266" s="2" t="s">
         <v>527</v>
       </c>
+      <c r="AK266" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="267" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A267" s="3">
         <v>44738.665040057866</v>
       </c>
@@ -31449,11 +32170,11 @@
       <c r="AI267" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="AJ267" s="2" t="s">
+      <c r="AJ267" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="268" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A268" s="3">
         <v>44739.984586006947</v>
       </c>
@@ -31562,8 +32283,11 @@
       <c r="AJ268" s="2" t="s">
         <v>530</v>
       </c>
+      <c r="AK268" s="2" t="s">
+        <v>617</v>
+      </c>
     </row>
-    <row r="269" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A269" s="3">
         <v>44740.421313680556</v>
       </c>
@@ -31669,11 +32393,11 @@
       <c r="AI269" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="AJ269" s="2" t="s">
+      <c r="AJ269" s="4" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="270" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A270" s="3">
         <v>44740.486668796293</v>
       </c>
@@ -31782,8 +32506,11 @@
       <c r="AJ270" s="2" t="s">
         <v>534</v>
       </c>
+      <c r="AK270" s="2" t="s">
+        <v>600</v>
+      </c>
     </row>
-    <row r="271" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A271" s="3">
         <v>44740.711242500001</v>
       </c>
@@ -31889,11 +32616,11 @@
       <c r="AI271" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="AJ271" s="2" t="s">
+      <c r="AJ271" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="272" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A272" s="3">
         <v>44740.811190532404</v>
       </c>
@@ -31999,11 +32726,12 @@
       <c r="AI272" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="AJ272" s="2" t="s">
+      <c r="AJ272" s="4" t="s">
         <v>537</v>
       </c>
+      <c r="AK272" s="2"/>
     </row>
-    <row r="273" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A273" s="3">
         <v>44741.521409131943</v>
       </c>
@@ -32112,8 +32840,11 @@
       <c r="AJ273" s="2" t="s">
         <v>539</v>
       </c>
+      <c r="AK273" s="2" t="s">
+        <v>616</v>
+      </c>
     </row>
-    <row r="274" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A274" s="3">
         <v>44741.525499467592</v>
       </c>
@@ -32219,11 +32950,11 @@
       <c r="AI274" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="AJ274" s="2" t="s">
+      <c r="AJ274" s="4" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="275" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A275" s="3">
         <v>44741.541521932872</v>
       </c>
@@ -32329,11 +33060,12 @@
       <c r="AI275" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="AJ275" s="2" t="s">
+      <c r="AJ275" s="4" t="s">
         <v>543</v>
       </c>
+      <c r="AK275" s="2"/>
     </row>
-    <row r="276" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A276" s="3">
         <v>44741.544849097219</v>
       </c>
@@ -32442,8 +33174,11 @@
       <c r="AJ276" s="2" t="s">
         <v>545</v>
       </c>
+      <c r="AK276" s="2" t="s">
+        <v>618</v>
+      </c>
     </row>
-    <row r="277" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A277" s="3">
         <v>44741.549618738427</v>
       </c>
@@ -32549,11 +33284,11 @@
       <c r="AI277" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="AJ277" s="2" t="s">
+      <c r="AJ277" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="278" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A278" s="3">
         <v>44741.552675185187</v>
       </c>
@@ -32662,8 +33397,11 @@
       <c r="AJ278" s="2" t="s">
         <v>548</v>
       </c>
+      <c r="AK278" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="279" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A279" s="3">
         <v>44741.571293298606</v>
       </c>
@@ -32772,8 +33510,11 @@
       <c r="AJ279" s="2" t="s">
         <v>550</v>
       </c>
+      <c r="AK279" s="2" t="s">
+        <v>625</v>
+      </c>
     </row>
-    <row r="280" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A280" s="3">
         <v>44741.571740671294</v>
       </c>
@@ -32882,8 +33623,14 @@
       <c r="AJ280" s="2" t="s">
         <v>552</v>
       </c>
+      <c r="AK280" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="AL280" s="2" t="s">
+        <v>600</v>
+      </c>
     </row>
-    <row r="281" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A281" s="3">
         <v>44741.583450138889</v>
       </c>
@@ -32992,8 +33739,17 @@
       <c r="AJ281" s="2" t="s">
         <v>554</v>
       </c>
+      <c r="AK281" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="AL281" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="AM281" s="5" t="s">
+        <v>629</v>
+      </c>
     </row>
-    <row r="282" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A282" s="3">
         <v>44741.603242442128</v>
       </c>
@@ -33099,11 +33855,12 @@
       <c r="AI282" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="AJ282" s="2" t="s">
+      <c r="AJ282" s="4" t="s">
         <v>556</v>
       </c>
+      <c r="AK282" s="2"/>
     </row>
-    <row r="283" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A283" s="3">
         <v>44741.638515150466</v>
       </c>
@@ -33212,8 +33969,11 @@
       <c r="AJ283" s="2" t="s">
         <v>558</v>
       </c>
+      <c r="AK283" s="2" t="s">
+        <v>597</v>
+      </c>
     </row>
-    <row r="284" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A284" s="3">
         <v>44741.658038194444</v>
       </c>
@@ -33319,11 +34079,12 @@
       <c r="AI284" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="AJ284" s="2" t="s">
+      <c r="AJ284" s="4" t="s">
         <v>560</v>
       </c>
+      <c r="AK284" s="2"/>
     </row>
-    <row r="285" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A285" s="3">
         <v>44741.722661527776</v>
       </c>
@@ -33429,11 +34190,11 @@
       <c r="AI285" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="AJ285" s="2" t="s">
+      <c r="AJ285" s="4" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="286" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A286" s="3">
         <v>44741.726033020837</v>
       </c>
@@ -33542,8 +34303,14 @@
       <c r="AJ286" s="2" t="s">
         <v>564</v>
       </c>
+      <c r="AK286" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AL286" s="2" t="s">
+        <v>628</v>
+      </c>
     </row>
-    <row r="287" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A287" s="3">
         <v>44741.748427152779</v>
       </c>
@@ -33652,8 +34419,11 @@
       <c r="AJ287" s="2" t="s">
         <v>566</v>
       </c>
+      <c r="AK287" s="2" t="s">
+        <v>620</v>
+      </c>
     </row>
-    <row r="288" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A288" s="3">
         <v>44741.779915046296</v>
       </c>
@@ -33759,11 +34529,11 @@
       <c r="AI288" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="AJ288" s="2" t="s">
+      <c r="AJ288" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="289" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A289" s="3">
         <v>44741.828575671301</v>
       </c>
@@ -33869,11 +34639,11 @@
       <c r="AI289" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="AJ289" s="2" t="s">
+      <c r="AJ289" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="290" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A290" s="3">
         <v>44742.352286956018</v>
       </c>
@@ -33982,8 +34752,11 @@
       <c r="AJ290" s="2" t="s">
         <v>570</v>
       </c>
+      <c r="AK290" s="2" t="s">
+        <v>628</v>
+      </c>
     </row>
-    <row r="291" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A291" s="3">
         <v>44742.445292349541</v>
       </c>
@@ -34092,8 +34865,11 @@
       <c r="AJ291" s="2" t="s">
         <v>572</v>
       </c>
+      <c r="AK291" s="2" t="s">
+        <v>599</v>
+      </c>
     </row>
-    <row r="292" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A292" s="3">
         <v>44742.507500324078</v>
       </c>
@@ -34202,8 +34978,11 @@
       <c r="AJ292" s="2" t="s">
         <v>574</v>
       </c>
+      <c r="AK292" s="2" t="s">
+        <v>614</v>
+      </c>
     </row>
-    <row r="293" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A293" s="3">
         <v>44742.50960449074</v>
       </c>
@@ -34309,11 +35088,11 @@
       <c r="AI293" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="AJ293" s="2" t="s">
+      <c r="AJ293" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="294" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A294" s="3">
         <v>44742.534232407408</v>
       </c>
@@ -34422,8 +35201,11 @@
       <c r="AJ294" s="2" t="s">
         <v>577</v>
       </c>
+      <c r="AK294" s="2" t="s">
+        <v>597</v>
+      </c>
     </row>
-    <row r="295" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A295" s="3">
         <v>44742.724200127312</v>
       </c>
@@ -34529,11 +35311,11 @@
       <c r="AI295" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="AJ295" s="2" t="s">
+      <c r="AJ295" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="296" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A296" s="3">
         <v>44742.735193414352</v>
       </c>
@@ -34642,8 +35424,11 @@
       <c r="AJ296" s="2" t="s">
         <v>580</v>
       </c>
+      <c r="AK296" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
-    <row r="297" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A297" s="3">
         <v>44742.850955324073</v>
       </c>
@@ -34752,8 +35537,11 @@
       <c r="AJ297" s="2" t="s">
         <v>582</v>
       </c>
+      <c r="AK297" s="2" t="s">
+        <v>629</v>
+      </c>
     </row>
-    <row r="298" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A298" s="3">
         <v>44747.32180445602</v>
       </c>
@@ -34859,11 +35647,11 @@
       <c r="AI298" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="AJ298" s="2" t="s">
+      <c r="AJ298" s="4" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="299" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A299" s="3">
         <v>44756.078680266204</v>
       </c>
@@ -34972,8 +35760,11 @@
       <c r="AJ299" s="2" t="s">
         <v>585</v>
       </c>
+      <c r="AK299" s="2" t="s">
+        <v>621</v>
+      </c>
     </row>
-    <row r="300" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A300" s="3">
         <v>44763.429490972223</v>
       </c>
@@ -35079,11 +35870,11 @@
       <c r="AI300" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="AJ300" s="2" t="s">
+      <c r="AJ300" s="4" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="301" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A301" s="3">
         <v>44766.709533854169</v>
       </c>
@@ -35192,8 +35983,13 @@
       <c r="AJ301" s="2" t="s">
         <v>589</v>
       </c>
+      <c r="AK301" s="2" t="s">
+        <v>594</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="AJ1:AM301"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>